<commit_message>
Update market data and stock dump
🤖 Generated with [Claude Code](https://claude.com/claude-code)

Co-Authored-By: Claude <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/dumps/Stocks/Bharat Coking Coal Ltd.xlsx
+++ b/dumps/Stocks/Bharat Coking Coal Ltd.xlsx
@@ -426,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AB5"/>
+  <dimension ref="A1:AB10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -574,39 +574,204 @@
     </row>
     <row r="5">
       <c r="A5" s="2" t="n">
+        <v>46059</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>NSE</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Buy</t>
+        </is>
+      </c>
+      <c r="D5" t="n">
+        <v>1</v>
+      </c>
+      <c r="E5" t="n">
+        <v>37.32</v>
+      </c>
+      <c r="F5" t="n">
+        <v>37.32</v>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>~</t>
+        </is>
+      </c>
+      <c r="J5">
+        <f>Index!$C$2</f>
+        <v/>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="2" t="n">
+        <v>46059</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>NSE</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Buy</t>
+        </is>
+      </c>
+      <c r="D6" t="n">
+        <v>99</v>
+      </c>
+      <c r="E6" t="n">
+        <v>37.31</v>
+      </c>
+      <c r="F6" t="n">
+        <v>3693.69</v>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>~</t>
+        </is>
+      </c>
+      <c r="J6">
+        <f>Index!$C$2</f>
+        <v/>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="2" t="n">
+        <v>46050</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>NSE</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>Buy</t>
+        </is>
+      </c>
+      <c r="D7" t="n">
+        <v>100</v>
+      </c>
+      <c r="E7" t="n">
+        <v>38.21</v>
+      </c>
+      <c r="F7" t="n">
+        <v>3821</v>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>~</t>
+        </is>
+      </c>
+      <c r="J7">
+        <f>Index!$C$2</f>
+        <v/>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="2" t="n">
+        <v>46049</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>NSE</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>Buy</t>
+        </is>
+      </c>
+      <c r="D8" t="n">
+        <v>100</v>
+      </c>
+      <c r="E8" t="n">
+        <v>35.88</v>
+      </c>
+      <c r="F8" t="n">
+        <v>3588</v>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>~</t>
+        </is>
+      </c>
+      <c r="J8">
+        <f>Index!$C$2</f>
+        <v/>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="2" t="n">
+        <v>46044</v>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>NSE</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>Buy</t>
+        </is>
+      </c>
+      <c r="D9" t="n">
+        <v>250</v>
+      </c>
+      <c r="E9" t="n">
+        <v>39.38</v>
+      </c>
+      <c r="F9" t="n">
+        <v>9845</v>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>~</t>
+        </is>
+      </c>
+      <c r="J9">
+        <f>Index!$C$2</f>
+        <v/>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="2" t="n">
         <v>46062</v>
       </c>
-      <c r="B5" t="inlineStr">
+      <c r="B10" t="inlineStr">
         <is>
           <t>NSE</t>
         </is>
       </c>
-      <c r="C5" t="inlineStr">
+      <c r="C10" t="inlineStr">
         <is>
           <t>Buy</t>
         </is>
       </c>
-      <c r="D5" t="n">
+      <c r="D10" t="n">
         <v>100</v>
       </c>
-      <c r="E5" t="n">
+      <c r="E10" t="n">
         <v>36.7</v>
       </c>
-      <c r="F5" t="n">
+      <c r="F10" t="n">
         <v>3695.58</v>
       </c>
-      <c r="G5" t="inlineStr">
+      <c r="G10" t="inlineStr">
         <is>
           <t>CN#252611665409</t>
         </is>
       </c>
-      <c r="H5" t="n">
+      <c r="H10" t="n">
         <v>3.67</v>
       </c>
-      <c r="I5" t="n">
+      <c r="I10" t="n">
         <v>21.91</v>
       </c>
-      <c r="J5">
+      <c r="J10">
         <f>Index!$C$2</f>
         <v/>
       </c>

</xml_diff>